<commit_message>
New and updated data
</commit_message>
<xml_diff>
--- a/Data/Sprague-uBiome Analysis.xlsx
+++ b/Data/Sprague-uBiome Analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="240" windowWidth="24600" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25000" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>May</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
   </si>
 </sst>
 </file>
@@ -157,13 +160,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -196,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="32">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -211,6 +216,7 @@
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -225,6 +231,7 @@
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
@@ -555,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F16"/>
+      <selection activeCell="G16" sqref="A2:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -566,7 +573,7 @@
     <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="1" customFormat="1">
+    <row r="2" spans="1:7" s="1" customFormat="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -580,9 +587,12 @@
       <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -598,11 +608,14 @@
       <c r="E3" s="3">
         <v>95382</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="3">
+        <v>136354</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -618,11 +631,14 @@
       <c r="E4" s="3">
         <v>42782</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="3">
+        <v>10750</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -638,11 +654,14 @@
       <c r="E5" s="3">
         <v>40977</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="3">
+        <v>13530</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -659,10 +678,13 @@
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -679,10 +701,13 @@
         <v>6269</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -698,11 +723,14 @@
       <c r="E8" s="3">
         <v>9571</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="3">
+        <v>2115</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -718,19 +746,23 @@
       <c r="E9" s="3">
         <v>66516</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="3">
+        <v>6919</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -749,17 +781,22 @@
         <f>E8/E9</f>
         <v>0.14389019183354382</v>
       </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="4">
+        <f>F8/F9</f>
+        <v>0.30568001156236452</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -775,11 +812,14 @@
       <c r="E13" s="3">
         <v>66114</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="3">
+        <v>17628</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -794,10 +834,13 @@
         <v>128</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -813,11 +856,14 @@
       <c r="E15" s="3">
         <v>24128</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="3">
+        <v>16747</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -833,7 +879,10 @@
       <c r="E16" s="3">
         <v>30543</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="3">
+        <v>132</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>